<commit_message>
add Test raport + logger
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ostol/Desktop/WSB-NLU/3_III SEMEST/Programowanie w JAVA/Laboratoria/PHPTravelsTest/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5457DE-44DC-724A-97B5-2EADADA303BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D737EDD2-7587-8D41-9AAB-B0B3E03874BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{BEE6D005-5C15-C04B-81FE-3132D3B20CAC}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{BEE6D005-5C15-C04B-81FE-3132D3B20CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -409,7 +409,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>